<commit_message>
Testverwachting structuurvisie aangepast; structuurvisie altijd doorlaten
</commit_message>
<xml_diff>
--- a/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch_TAM-uitgebreid.xlsx
+++ b/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch_TAM-uitgebreid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtinggeonovum.sharepoint.com/sites/msteams_a07e8e/Gedeelde documenten/General/22013 TAM-IMRO verbreed gebruik/AanpassingValidator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijsk\Documents\GitHub\imro-dev\Overgangsrecht+TAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="8_{6AF6F881-74FA-4612-8D28-EBD4989D30F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00017A2A-6D97-49FB-B66A-CD4F8D84AFDF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DF9043-A2F9-4BD1-8B7C-265B62A0DDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Test - XSLT1 - Kadaster" sheetId="4" r:id="rId1"/>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C8936-D7D1-4C1D-960D-9AD61970D693}">
   <dimension ref="A1:FC51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1746,8 +1746,8 @@
       <c r="C38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>30</v>
+      <c r="D38" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -1927,17 +1927,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ab01c9f7-308e-412a-8b6b-2a38868f1fe8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f5714f12-861a-48fb-8033-d35a907f947e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063B796D0CB608148ADB6A3FE6184D975" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="71d6b85c0b6e09903bf280259070e852">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ab01c9f7-308e-412a-8b6b-2a38868f1fe8" xmlns:ns3="f5714f12-861a-48fb-8033-d35a907f947e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f26ee0e1d009816e1c8af2a8a71dce8" ns2:_="" ns3:_="">
     <xsd:import namespace="ab01c9f7-308e-412a-8b6b-2a38868f1fe8"/>
@@ -2126,6 +2115,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ab01c9f7-308e-412a-8b6b-2a38868f1fe8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f5714f12-861a-48fb-8033-d35a907f947e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2136,17 +2136,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DD17D3-045C-46B8-BB98-00D1B5119EE5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ab01c9f7-308e-412a-8b6b-2a38868f1fe8"/>
-    <ds:schemaRef ds:uri="f5714f12-861a-48fb-8033-d35a907f947e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58DE8008-C1B9-4D83-B2C3-04BDD37EF824}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2165,6 +2154,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DD17D3-045C-46B8-BB98-00D1B5119EE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ab01c9f7-308e-412a-8b6b-2a38868f1fe8"/>
+    <ds:schemaRef ds:uri="f5714f12-861a-48fb-8033-d35a907f947e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955549FB-6958-4E07-8677-91C492AD0DEA}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Ow+TAMuitgebreid opgenomen in schematron
1) Validatieregels voor Ow + TAM uitgebreid geïmplementeerd in apart schematron TAM.sch

2) Elke GML in validatie_testbestanden_TAM-uitgebreid getest: testresultaat conform verwachting. Testresultaat toegevoegd aan kolom E 'testresultaat na ontwikkeling'.

3) <iso:pattern id="OwTAMuitgebreid"> toegevoegd aan additional-validator-rules-2012v0.08-b-RC.sch
</commit_message>
<xml_diff>
--- a/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch_TAM-uitgebreid.xlsx
+++ b/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch_TAM-uitgebreid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijsk\Documents\GitHub\imro-dev\Overgangsrecht+TAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Github\Geonovum\imro-dev\Overgangsrecht+TAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82985CD-6890-471B-8B0A-13C241DA276E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3520C6-653D-4201-886C-31C71FDBC7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Test - XSLT1 - Kadaster" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="106">
   <si>
     <t>AMVB</t>
   </si>
@@ -313,6 +313,48 @@
   </si>
   <si>
     <t>1d: datum na_IOW_geconsolideerd  NL.IMRO.0202.EPP976-0301</t>
+  </si>
+  <si>
+    <t>Validatie succesvol</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0000.BZKam11Barro-3025, type = imro:Besluitgebied_A: Fout in typePlan -&gt; Als typePlan is 'amvb' of 'regeling' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'amvb' of 'regeling'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0106.99BHV2020180B-C001, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'beheersverordening' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'beheersverordening'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.1930.BPRaadhuislaanSP-1001, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'bestemmingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld' of 'geconsolideerd', tenzij naam begint met 'TAM-omgevingsplan '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0855.EXP2021001-b001, type = imro:Besluitgebied_X: Fout in planstatus -&gt; Als imro:typePlan is 'exploitatieplan' en datum is groter dan of gelijk aan 2023-01-01, dan mag planstatus niet zijn 'ontwerp', 'concept' of 'voorontwerp'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0000.EZKip18GaswTern-2001, type = imro:Bestemmingsplangebied: Fout in typePlan -&gt; Als typePlan is 'inpassingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'inpassingsplan', tenzij naam begint met 'TAM-projectbesluit '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id , type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'projectbesluit' of 'tijdelijke ontheffing buitenplans' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'projectbesluit' of 'tijdelijke ontheffing buitenplans'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.9923.phVerordening006B-va01, type = imro:Besluitgebied_P: Fout in typePlan -&gt; Als typePlan is 'provinciale verordening' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'provinciale verordening', tenzij naam begint met 'TAM-omgevingsverordening '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.9926.RA0318SLAPPEDEL8A-VA01, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'reactieve aanwijzing' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'reactieve aanwijzing', tenzij naam begint met 'TAM-reactieve interventie '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0000.BZKmr11Rarro-3050, type = imro:Besluitgebied_A: Fout in typePlan -&gt; Als typePlan is 'amvb' of 'regeling' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'amvb' of 'regeling'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0345.UPDeOntmoetingDp7-ow01, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'uitwerkingsplan' of 'wijzigingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0202.VBB985-0301, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typeplan is voorbereidingsbesluit en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'voorbereidingsbesluit', tenzij naam begint met 'TAM-voorbereidingsbesluit '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0302.WI01031-ow01, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'uitwerkingsplan' of 'wijzigingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld'.</t>
+  </si>
+  <si>
+    <t>Testresultaat na ontwikkeling</t>
   </si>
 </sst>
 </file>
@@ -416,43 +458,56 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
@@ -769,24 +824,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C8936-D7D1-4C1D-960D-9AD61970D693}">
-  <dimension ref="A1:FC52"/>
+  <dimension ref="A1:FD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.44140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="59.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="78.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="59.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:160" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -798,13 +854,16 @@
         <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:159" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:160" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -817,8 +876,10 @@
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -972,8 +1033,9 @@
       <c r="FA2" s="4"/>
       <c r="FB2" s="4"/>
       <c r="FC2" s="4"/>
-    </row>
-    <row r="3" spans="1:159" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="FD2" s="4"/>
+    </row>
+    <row r="3" spans="1:160" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -984,8 +1046,10 @@
       <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="9"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1139,176 +1203,216 @@
       <c r="FA3" s="4"/>
       <c r="FB3" s="4"/>
       <c r="FC3" s="4"/>
-    </row>
-    <row r="4" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="FD3" s="4"/>
+    </row>
+    <row r="4" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:160" ht="150" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:160" ht="150" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:160" ht="210" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E10" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:160" ht="210" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:160" ht="210" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E12" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:160" ht="180" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E16" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
@@ -1318,9 +1422,12 @@
       <c r="D17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>90</v>
       </c>
@@ -1330,24 +1437,30 @@
       <c r="D18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>14</v>
       </c>
@@ -1357,48 +1470,60 @@
       <c r="D20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:160" ht="180" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E23" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
@@ -1408,36 +1533,45 @@
       <c r="D24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>85</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E25" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="1:159" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:160" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>14</v>
@@ -1448,8 +1582,10 @@
       <c r="D27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="7"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1603,233 +1739,285 @@
       <c r="FA27" s="4"/>
       <c r="FB27" s="4"/>
       <c r="FC27" s="4"/>
-    </row>
-    <row r="28" spans="1:159" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="FD27" s="4"/>
+    </row>
+    <row r="28" spans="1:160" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="15" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E28" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:160" ht="195" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E29" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>53</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:160" ht="195" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:159" x14ac:dyDescent="0.3">
+      <c r="E31" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:160" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>87</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>55</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E34" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>89</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E36" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E37" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="10" t="s">
         <v>59</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E38" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="10" t="s">
         <v>60</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E39" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="10" t="s">
         <v>61</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E40" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E41" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E42" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="10" t="s">
         <v>64</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E43" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E44" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>11</v>
       </c>
@@ -1839,98 +2027,122 @@
       <c r="D45" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E45" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="13" t="s">
+      <c r="E46" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E47" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="16"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="10" t="s">
         <v>73</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="6"/>
+      <c r="E52" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1939,14 +2151,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ab01c9f7-308e-412a-8b6b-2a38868f1fe8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f5714f12-861a-48fb-8033-d35a907f947e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2139,21 +2349,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ab01c9f7-308e-412a-8b6b-2a38868f1fe8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f5714f12-861a-48fb-8033-d35a907f947e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DD17D3-045C-46B8-BB98-00D1B5119EE5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955549FB-6958-4E07-8677-91C492AD0DEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ab01c9f7-308e-412a-8b6b-2a38868f1fe8"/>
-    <ds:schemaRef ds:uri="f5714f12-861a-48fb-8033-d35a907f947e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2178,9 +2387,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955549FB-6958-4E07-8677-91C492AD0DEA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DD17D3-045C-46B8-BB98-00D1B5119EE5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ab01c9f7-308e-412a-8b6b-2a38868f1fe8"/>
+    <ds:schemaRef ds:uri="f5714f12-861a-48fb-8033-d35a907f947e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Testresultaat additional-validator-rules-2012v0.08-b-RC.sch op pilot.RPnl
</commit_message>
<xml_diff>
--- a/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch_TAM-uitgebreid.xlsx
+++ b/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch_TAM-uitgebreid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Github\Geonovum\imro-dev\Overgangsrecht+TAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijsk\Documents\GitHub\imro-dev\Overgangsrecht+TAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3520C6-653D-4201-886C-31C71FDBC7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590698FA-8C11-4A79-BA28-71C03E36C701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Test - XSLT1 - Kadaster" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="112">
   <si>
     <t>AMVB</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>Testresultaat na ontwikkeling</t>
+  </si>
+  <si>
+    <t>1_IOW_toestaan_planstatus_ontwerp</t>
+  </si>
+  <si>
+    <t>1: validatie_IOW_toestaan_planstatus_ontwerp vóór IWT</t>
+  </si>
+  <si>
+    <t>Testbestand niet correct</t>
+  </si>
+  <si>
+    <t>Onterecht doorgelaten</t>
+  </si>
+  <si>
+    <t>(Planobject gml:id = NL.IMRO.0202.EPP976-0301 , type = imro:Besluitgebied_X ) Foutcode RPA15: Attribuut besluitnummer en verwijzingNaarVaststellingsbesluit alleen toegestaan en verplicht vanaf planstatus = vastgesteld of onherroepelijk. (Huidige waarde planstatus: geconsolideerd ) Zie constraint b4, c5, e5, e13, e19 (afhankelijk van het type planobject) van IMRO2012.pdf paragraaf 8.4.</t>
+  </si>
+  <si>
+    <t>Testbestand lijkt in orde</t>
   </si>
 </sst>
 </file>
@@ -399,7 +417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +443,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,7 +482,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -478,13 +502,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -496,9 +514,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -507,6 +522,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -824,25 +845,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C8936-D7D1-4C1D-960D-9AD61970D693}">
-  <dimension ref="A1:FD52"/>
+  <dimension ref="A1:FD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="78.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="16" customWidth="1"/>
-    <col min="7" max="7" width="59.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="29.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:160" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:160" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -863,7 +884,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:160" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:160" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -879,7 +900,9 @@
       <c r="E2" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1035,7 +1058,7 @@
       <c r="FC2" s="4"/>
       <c r="FD2" s="4"/>
     </row>
-    <row r="3" spans="1:160" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:160" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -1049,7 +1072,9 @@
       <c r="E3" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1205,14 +1230,14 @@
       <c r="FC3" s="4"/>
       <c r="FD3" s="4"/>
     </row>
-    <row r="4" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:160" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1221,31 +1246,35 @@
       <c r="E4" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:160" ht="150" x14ac:dyDescent="0.25">
+      <c r="F4" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:160" ht="144" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:160" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:160" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -1254,895 +1283,1013 @@
       <c r="E6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:160" ht="150" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:160" ht="144" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:160" x14ac:dyDescent="0.25">
+      <c r="F7" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:160" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:160" ht="210" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:160" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:160" ht="210" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="F11" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:160" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:160" ht="210" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="F12" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:160" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="F13" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:160" ht="180" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="D16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:160" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E17" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="F17" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="D18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="D19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="D20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="D21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="D22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:160" ht="180" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="D23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:160" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D24" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E24" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="F24" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="D25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="B26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="D26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:160" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4" t="s">
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:160" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
-      <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
-      <c r="AG27" s="4"/>
-      <c r="AH27" s="4"/>
-      <c r="AI27" s="4"/>
-      <c r="AJ27" s="4"/>
-      <c r="AK27" s="4"/>
-      <c r="AL27" s="4"/>
-      <c r="AM27" s="4"/>
-      <c r="AN27" s="4"/>
-      <c r="AO27" s="4"/>
-      <c r="AP27" s="4"/>
-      <c r="AQ27" s="4"/>
-      <c r="AR27" s="4"/>
-      <c r="AS27" s="4"/>
-      <c r="AT27" s="4"/>
-      <c r="AU27" s="4"/>
-      <c r="AV27" s="4"/>
-      <c r="AW27" s="4"/>
-      <c r="AX27" s="4"/>
-      <c r="AY27" s="4"/>
-      <c r="AZ27" s="4"/>
-      <c r="BA27" s="4"/>
-      <c r="BB27" s="4"/>
-      <c r="BC27" s="4"/>
-      <c r="BD27" s="4"/>
-      <c r="BE27" s="4"/>
-      <c r="BF27" s="4"/>
-      <c r="BG27" s="4"/>
-      <c r="BH27" s="4"/>
-      <c r="BI27" s="4"/>
-      <c r="BJ27" s="4"/>
-      <c r="BK27" s="4"/>
-      <c r="BL27" s="4"/>
-      <c r="BM27" s="4"/>
-      <c r="BN27" s="4"/>
-      <c r="BO27" s="4"/>
-      <c r="BP27" s="4"/>
-      <c r="BQ27" s="4"/>
-      <c r="BR27" s="4"/>
-      <c r="BS27" s="4"/>
-      <c r="BT27" s="4"/>
-      <c r="BU27" s="4"/>
-      <c r="BV27" s="4"/>
-      <c r="BW27" s="4"/>
-      <c r="BX27" s="4"/>
-      <c r="BY27" s="4"/>
-      <c r="BZ27" s="4"/>
-      <c r="CA27" s="4"/>
-      <c r="CB27" s="4"/>
-      <c r="CC27" s="4"/>
-      <c r="CD27" s="4"/>
-      <c r="CE27" s="4"/>
-      <c r="CF27" s="4"/>
-      <c r="CG27" s="4"/>
-      <c r="CH27" s="4"/>
-      <c r="CI27" s="4"/>
-      <c r="CJ27" s="4"/>
-      <c r="CK27" s="4"/>
-      <c r="CL27" s="4"/>
-      <c r="CM27" s="4"/>
-      <c r="CN27" s="4"/>
-      <c r="CO27" s="4"/>
-      <c r="CP27" s="4"/>
-      <c r="CQ27" s="4"/>
-      <c r="CR27" s="4"/>
-      <c r="CS27" s="4"/>
-      <c r="CT27" s="4"/>
-      <c r="CU27" s="4"/>
-      <c r="CV27" s="4"/>
-      <c r="CW27" s="4"/>
-      <c r="CX27" s="4"/>
-      <c r="CY27" s="4"/>
-      <c r="CZ27" s="4"/>
-      <c r="DA27" s="4"/>
-      <c r="DB27" s="4"/>
-      <c r="DC27" s="4"/>
-      <c r="DD27" s="4"/>
-      <c r="DE27" s="4"/>
-      <c r="DF27" s="4"/>
-      <c r="DG27" s="4"/>
-      <c r="DH27" s="4"/>
-      <c r="DI27" s="4"/>
-      <c r="DJ27" s="4"/>
-      <c r="DK27" s="4"/>
-      <c r="DL27" s="4"/>
-      <c r="DM27" s="4"/>
-      <c r="DN27" s="4"/>
-      <c r="DO27" s="4"/>
-      <c r="DP27" s="4"/>
-      <c r="DQ27" s="4"/>
-      <c r="DR27" s="4"/>
-      <c r="DS27" s="4"/>
-      <c r="DT27" s="4"/>
-      <c r="DU27" s="4"/>
-      <c r="DV27" s="4"/>
-      <c r="DW27" s="4"/>
-      <c r="DX27" s="4"/>
-      <c r="DY27" s="4"/>
-      <c r="DZ27" s="4"/>
-      <c r="EA27" s="4"/>
-      <c r="EB27" s="4"/>
-      <c r="EC27" s="4"/>
-      <c r="ED27" s="4"/>
-      <c r="EE27" s="4"/>
-      <c r="EF27" s="4"/>
-      <c r="EG27" s="4"/>
-      <c r="EH27" s="4"/>
-      <c r="EI27" s="4"/>
-      <c r="EJ27" s="4"/>
-      <c r="EK27" s="4"/>
-      <c r="EL27" s="4"/>
-      <c r="EM27" s="4"/>
-      <c r="EN27" s="4"/>
-      <c r="EO27" s="4"/>
-      <c r="EP27" s="4"/>
-      <c r="EQ27" s="4"/>
-      <c r="ER27" s="4"/>
-      <c r="ES27" s="4"/>
-      <c r="ET27" s="4"/>
-      <c r="EU27" s="4"/>
-      <c r="EV27" s="4"/>
-      <c r="EW27" s="4"/>
-      <c r="EX27" s="4"/>
-      <c r="EY27" s="4"/>
-      <c r="EZ27" s="4"/>
-      <c r="FA27" s="4"/>
-      <c r="FB27" s="4"/>
-      <c r="FC27" s="4"/>
-      <c r="FD27" s="4"/>
-    </row>
-    <row r="28" spans="1:160" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="D28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="4"/>
+      <c r="AI28" s="4"/>
+      <c r="AJ28" s="4"/>
+      <c r="AK28" s="4"/>
+      <c r="AL28" s="4"/>
+      <c r="AM28" s="4"/>
+      <c r="AN28" s="4"/>
+      <c r="AO28" s="4"/>
+      <c r="AP28" s="4"/>
+      <c r="AQ28" s="4"/>
+      <c r="AR28" s="4"/>
+      <c r="AS28" s="4"/>
+      <c r="AT28" s="4"/>
+      <c r="AU28" s="4"/>
+      <c r="AV28" s="4"/>
+      <c r="AW28" s="4"/>
+      <c r="AX28" s="4"/>
+      <c r="AY28" s="4"/>
+      <c r="AZ28" s="4"/>
+      <c r="BA28" s="4"/>
+      <c r="BB28" s="4"/>
+      <c r="BC28" s="4"/>
+      <c r="BD28" s="4"/>
+      <c r="BE28" s="4"/>
+      <c r="BF28" s="4"/>
+      <c r="BG28" s="4"/>
+      <c r="BH28" s="4"/>
+      <c r="BI28" s="4"/>
+      <c r="BJ28" s="4"/>
+      <c r="BK28" s="4"/>
+      <c r="BL28" s="4"/>
+      <c r="BM28" s="4"/>
+      <c r="BN28" s="4"/>
+      <c r="BO28" s="4"/>
+      <c r="BP28" s="4"/>
+      <c r="BQ28" s="4"/>
+      <c r="BR28" s="4"/>
+      <c r="BS28" s="4"/>
+      <c r="BT28" s="4"/>
+      <c r="BU28" s="4"/>
+      <c r="BV28" s="4"/>
+      <c r="BW28" s="4"/>
+      <c r="BX28" s="4"/>
+      <c r="BY28" s="4"/>
+      <c r="BZ28" s="4"/>
+      <c r="CA28" s="4"/>
+      <c r="CB28" s="4"/>
+      <c r="CC28" s="4"/>
+      <c r="CD28" s="4"/>
+      <c r="CE28" s="4"/>
+      <c r="CF28" s="4"/>
+      <c r="CG28" s="4"/>
+      <c r="CH28" s="4"/>
+      <c r="CI28" s="4"/>
+      <c r="CJ28" s="4"/>
+      <c r="CK28" s="4"/>
+      <c r="CL28" s="4"/>
+      <c r="CM28" s="4"/>
+      <c r="CN28" s="4"/>
+      <c r="CO28" s="4"/>
+      <c r="CP28" s="4"/>
+      <c r="CQ28" s="4"/>
+      <c r="CR28" s="4"/>
+      <c r="CS28" s="4"/>
+      <c r="CT28" s="4"/>
+      <c r="CU28" s="4"/>
+      <c r="CV28" s="4"/>
+      <c r="CW28" s="4"/>
+      <c r="CX28" s="4"/>
+      <c r="CY28" s="4"/>
+      <c r="CZ28" s="4"/>
+      <c r="DA28" s="4"/>
+      <c r="DB28" s="4"/>
+      <c r="DC28" s="4"/>
+      <c r="DD28" s="4"/>
+      <c r="DE28" s="4"/>
+      <c r="DF28" s="4"/>
+      <c r="DG28" s="4"/>
+      <c r="DH28" s="4"/>
+      <c r="DI28" s="4"/>
+      <c r="DJ28" s="4"/>
+      <c r="DK28" s="4"/>
+      <c r="DL28" s="4"/>
+      <c r="DM28" s="4"/>
+      <c r="DN28" s="4"/>
+      <c r="DO28" s="4"/>
+      <c r="DP28" s="4"/>
+      <c r="DQ28" s="4"/>
+      <c r="DR28" s="4"/>
+      <c r="DS28" s="4"/>
+      <c r="DT28" s="4"/>
+      <c r="DU28" s="4"/>
+      <c r="DV28" s="4"/>
+      <c r="DW28" s="4"/>
+      <c r="DX28" s="4"/>
+      <c r="DY28" s="4"/>
+      <c r="DZ28" s="4"/>
+      <c r="EA28" s="4"/>
+      <c r="EB28" s="4"/>
+      <c r="EC28" s="4"/>
+      <c r="ED28" s="4"/>
+      <c r="EE28" s="4"/>
+      <c r="EF28" s="4"/>
+      <c r="EG28" s="4"/>
+      <c r="EH28" s="4"/>
+      <c r="EI28" s="4"/>
+      <c r="EJ28" s="4"/>
+      <c r="EK28" s="4"/>
+      <c r="EL28" s="4"/>
+      <c r="EM28" s="4"/>
+      <c r="EN28" s="4"/>
+      <c r="EO28" s="4"/>
+      <c r="EP28" s="4"/>
+      <c r="EQ28" s="4"/>
+      <c r="ER28" s="4"/>
+      <c r="ES28" s="4"/>
+      <c r="ET28" s="4"/>
+      <c r="EU28" s="4"/>
+      <c r="EV28" s="4"/>
+      <c r="EW28" s="4"/>
+      <c r="EX28" s="4"/>
+      <c r="EY28" s="4"/>
+      <c r="EZ28" s="4"/>
+      <c r="FA28" s="4"/>
+      <c r="FB28" s="4"/>
+      <c r="FC28" s="4"/>
+      <c r="FD28" s="4"/>
+    </row>
+    <row r="29" spans="1:160" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C29" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:160" ht="195" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="D29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:160" ht="144" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E30" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="F30" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:160" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:160" ht="195" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="D31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:160" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C32" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E32" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="F32" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="D33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="D34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C35" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D35" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E35" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+      <c r="F35" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C36" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="D36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="D37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="B38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D38" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E38" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="F38" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="D39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="D40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C41" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+      <c r="D41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C42" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D42" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E42" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="F42" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C43" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+      <c r="D43" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C44" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="D44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C45" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D45" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E45" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="F45" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="D46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C47" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+      <c r="D47" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C48" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D48" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E48" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="16"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="F48" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C49" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="D49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C50" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+      <c r="D50" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C51" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="D51" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="B52" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C52" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D52" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F51" s="7"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="F52" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C53" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F52" s="7"/>
+      <c r="D53" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2151,15 +2298,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063B796D0CB608148ADB6A3FE6184D975" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="71d6b85c0b6e09903bf280259070e852">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ab01c9f7-308e-412a-8b6b-2a38868f1fe8" xmlns:ns3="f5714f12-861a-48fb-8033-d35a907f947e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f26ee0e1d009816e1c8af2a8a71dce8" ns2:_="" ns3:_="">
     <xsd:import namespace="ab01c9f7-308e-412a-8b6b-2a38868f1fe8"/>
@@ -2348,6 +2486,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2360,14 +2507,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955549FB-6958-4E07-8677-91C492AD0DEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58DE8008-C1B9-4D83-B2C3-04BDD37EF824}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2386,6 +2525,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955549FB-6958-4E07-8677-91C492AD0DEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DD17D3-045C-46B8-BB98-00D1B5119EE5}">
   <ds:schemaRefs>

</xml_diff>